<commit_message>
Added Processes with static and dynamic steps.
</commit_message>
<xml_diff>
--- a/src/Starter/wwwroot/uploads/tests/9/GeneratedForStarter Test.xlsx
+++ b/src/Starter/wwwroot/uploads/tests/9/GeneratedForStarter Test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>STEP_ID</t>
   </si>
@@ -41,25 +41,28 @@
     <t>Navigate</t>
   </si>
   <si>
+    <t>asd</t>
+  </si>
+  <si>
     <t>http://www.google.co.uk</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>lst-ib</t>
+  </si>
+  <si>
+    <t>Click by id</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>Click</t>
-  </si>
-  <si>
-    <t>lst-ib</t>
-  </si>
-  <si>
-    <t>Click by id</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Set</t>
   </si>
   <si>
     <t>//*[@id="lst-ib"]</t>
@@ -185,91 +188,94 @@
       <c r="B3" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="E3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>